<commit_message>
add excel upload(new, modify) and download in /myparts
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/tempxls/개발자테스트아이디.xlsx
+++ b/src/main/webapp/resources/tempxls/개발자테스트아이디.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="120" yWindow="90" windowWidth="16125" windowHeight="5595"/>
   </bookViews>
   <sheets>
-    <sheet name="출고요청" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="파츠관리" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>LGIT P/N</t>
   </si>
@@ -24,87 +25,64 @@
   </si>
   <si>
     <t>프로젝트코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2LL2N5BA11K-R</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>LQP03TN2N5B02D</t>
+  </si>
+  <si>
+    <t>MURATA ELEKTRONIK</t>
+  </si>
+  <si>
+    <t>S1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>재고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>위치</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Maker</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출고요청수량</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파츠 재고확인/출고요청용 시트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>단가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(머릿글행 임의변경 금지, 노란색열만 처리함)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>개발담당자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>부서</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시작담당자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TESTPRJ002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>개발자시험용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>asdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(헤더 임의변경 금지)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>TESTPRJA</t>
-  </si>
-  <si>
-    <t>개발자테스트아이디</t>
-  </si>
-  <si>
-    <t>전장부품</t>
-  </si>
-  <si>
-    <t>출고담당자시험용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신규 파츠 등록용 시트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TESTPRJA</t>
+  </si>
+  <si>
+    <t>kdj239/392</t>
+  </si>
+  <si>
+    <t>alv9djemf</t>
+  </si>
+  <si>
+    <t>MKr</t>
+  </si>
+  <si>
+    <t>3층 A</t>
   </si>
   <si>
     <t>2FTS00096A</t>
@@ -119,9 +97,6 @@
     <t>S1</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>2FTS00093A</t>
   </si>
   <si>
@@ -182,21 +157,17 @@
     <t>GRM033R71E471KA01D</t>
   </si>
   <si>
-    <t>MURATA ELEKTRONIK</t>
-  </si>
-  <si>
     <t>2LL2N5BA11K-R</t>
-  </si>
-  <si>
-    <t>LQP03TN2N5B02D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="10">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,19 +177,62 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="14"/>
@@ -257,21 +271,8 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF555555"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF555555"/>
-      <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,14 +285,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -314,9 +309,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -324,70 +337,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -683,396 +669,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="4" customWidth="true" width="16.125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="12.375" collapsed="false"/>
+    <col min="3" max="7" customWidth="true" width="9.875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:11">
+    <row r="1" spans="1:8" ht="18.75">
+      <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="F3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="27">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10.0</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.2130000591278076</v>
-      </c>
-      <c r="I5" t="n">
-        <v>530.0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="G5" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="n">
+        <v>530.0</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.210999995470047</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3000.0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
+      <c r="G6" t="n">
+        <v>1.2130000591278076</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3000.0</v>
+      </c>
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="n">
-        <v>351.1210021972656</v>
-      </c>
-      <c r="I7" t="n">
-        <v>4450.0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" t="s">
-        <v>28</v>
+      <c r="G7" t="n">
+        <v>0.210999995470047</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4450.0</v>
+      </c>
+      <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" t="n">
-        <v>53.21229934692383</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2260.0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" t="s">
-        <v>28</v>
+      <c r="G8" t="n">
+        <v>351.1210021972656</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2260.0</v>
+      </c>
+      <c r="F9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.12309999763965607</v>
-      </c>
-      <c r="I9" t="n">
-        <v>768.0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" t="s">
-        <v>28</v>
+      <c r="G9" t="n">
+        <v>53.21229934692383</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="n">
+        <v>768.0</v>
+      </c>
+      <c r="F10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.12399999797344208</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1275.0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" t="s">
-        <v>28</v>
+      <c r="G10" t="n">
+        <v>0.12309999763965607</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1275.0</v>
+      </c>
+      <c r="F11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.352400004863739</v>
-      </c>
-      <c r="I11" t="n">
-        <v>2200.0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" t="s">
-        <v>28</v>
+      <c r="G11" t="n">
+        <v>0.12399999797344208</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2200.0</v>
+      </c>
+      <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.15600000321865082</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1560.0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K12" t="s">
-        <v>28</v>
+      <c r="G12" t="n">
+        <v>0.352400004863739</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1560.0</v>
+      </c>
+      <c r="F13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" t="n">
+      <c r="G13" t="n">
+        <v>0.15600000321865082</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.12300000339746475</v>
       </c>
-      <c r="I13" t="n">
-        <v>4000.0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -1086,7 +969,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify ppt file for user guide
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/tempxls/개발자테스트아이디.xlsx
+++ b/src/main/webapp/resources/tempxls/개발자테스트아이디.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="180">
   <si>
     <t>LGIT P/N</t>
   </si>
@@ -79,33 +79,183 @@
     <t>출고담당자시험용</t>
   </si>
   <si>
-    <t>kdj239/392</t>
-  </si>
-  <si>
-    <t>alv9djemf</t>
-  </si>
-  <si>
-    <t>MKr</t>
-  </si>
-  <si>
-    <t>3층 A</t>
+    <t>2CAC01209A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H2R0BA01</t>
+  </si>
+  <si>
+    <t>MURATA ELEKTRONIK</t>
+  </si>
+  <si>
+    <t>S1</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>2CAC01231A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H2R5BA01</t>
+  </si>
+  <si>
+    <t>2CAC01187A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR60WA01</t>
+  </si>
+  <si>
+    <t>2LL2N7BA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN2N7B02D</t>
+  </si>
+  <si>
+    <t>2FTS00105A</t>
+  </si>
+  <si>
+    <t>SAFFB806MFA0F1B</t>
+  </si>
+  <si>
+    <t>2DIT00095A</t>
+  </si>
+  <si>
+    <t>VCUT05E1-SD0</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>2FTZ00032A</t>
+  </si>
+  <si>
+    <t>HHM22106B1</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>2FTS00068A</t>
+  </si>
+  <si>
+    <t>SAWFD1G84BH0F0A</t>
+  </si>
+  <si>
+    <t>2LL3N4BA11K-R</t>
+  </si>
+  <si>
+    <t>LQP03TN3N4B02D</t>
+  </si>
+  <si>
+    <t>2LL3N2BA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN3N2B02D</t>
+  </si>
+  <si>
+    <t>2ICL00079A</t>
+  </si>
+  <si>
+    <t>SKY77767</t>
+  </si>
+  <si>
+    <t>SKYWORKS SOLUTIONS</t>
+  </si>
+  <si>
+    <t>2FTS00065A</t>
+  </si>
+  <si>
+    <t>F6QA2G535H2JG</t>
+  </si>
+  <si>
+    <t>TAIYO YUDEN</t>
+  </si>
+  <si>
+    <t>2FTS00064A</t>
+  </si>
+  <si>
+    <t>F6QG2G655P2KE</t>
+  </si>
+  <si>
+    <t>2FTD00027A</t>
+  </si>
+  <si>
+    <t>D6HN2G655BN59C</t>
+  </si>
+  <si>
+    <t>2CAC00828A</t>
+  </si>
+  <si>
+    <t>GRM0335C1E8R0BA01D</t>
+  </si>
+  <si>
+    <t>2FTS00099A</t>
+  </si>
+  <si>
+    <t>F5QA806M0M2QE</t>
+  </si>
+  <si>
+    <t>2FTS00098A</t>
+  </si>
+  <si>
+    <t>SAYFH806MCA0F1B</t>
+  </si>
+  <si>
+    <t>2FTS00097A</t>
+  </si>
+  <si>
+    <t>F5QA847M0M2QR</t>
+  </si>
+  <si>
+    <t>2ICL00157A</t>
+  </si>
+  <si>
+    <t>SKY77736</t>
+  </si>
+  <si>
+    <t>2CAC01046A</t>
+  </si>
+  <si>
+    <t>GRM0335C1E1R0BA01D</t>
+  </si>
+  <si>
+    <t>2CAC01039A</t>
+  </si>
+  <si>
+    <t>GRM0335C1E3R3BA01D</t>
+  </si>
+  <si>
+    <t>2LL9N1HA11K-R</t>
+  </si>
+  <si>
+    <t>LQP03TN9N1H02D</t>
+  </si>
+  <si>
+    <t>2RSC01181A</t>
+  </si>
+  <si>
+    <t>RK73H1HTTC6191F</t>
+  </si>
+  <si>
+    <t>KOA CORPORATION NAGANO</t>
+  </si>
+  <si>
+    <t>2FTC00144A</t>
+  </si>
+  <si>
+    <t>DLU-1608-25GS1-A2-AT</t>
+  </si>
+  <si>
+    <t>MAGLAYERS</t>
+  </si>
+  <si>
     <t>2FTS00096A</t>
   </si>
   <si>
     <t>F6HF2G441AF46</t>
   </si>
   <si>
-    <t>TAIYO YUDEN</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t>2FTS00093A</t>
   </si>
   <si>
@@ -121,18 +271,12 @@
     <t>DLU-2012-25GS1-A1-AT</t>
   </si>
   <si>
-    <t>MAGLAYERS</t>
-  </si>
-  <si>
     <t>2FTP00015A</t>
   </si>
   <si>
     <t>DPX165950DT-8126A1</t>
   </si>
   <si>
-    <t>TDK</t>
-  </si>
-  <si>
     <t>2ICZ00186A</t>
   </si>
   <si>
@@ -166,7 +310,256 @@
     <t>GRM033R71E471KA01D</t>
   </si>
   <si>
-    <t>MURATA ELEKTRONIK</t>
+    <t>2CAC00926A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H6R2BA01D</t>
+  </si>
+  <si>
+    <t>2CAC00824A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H2R2BA01D</t>
+  </si>
+  <si>
+    <t>2FTS00062A</t>
+  </si>
+  <si>
+    <t>F5QG751M0P2KR</t>
+  </si>
+  <si>
+    <t>2LP6N2HA50K-F</t>
+  </si>
+  <si>
+    <t>LQP03TN6N2H02D</t>
+  </si>
+  <si>
+    <t>2ICZ00044A</t>
+  </si>
+  <si>
+    <t>SKY13421-486LF</t>
+  </si>
+  <si>
+    <t>2FTS00061A</t>
+  </si>
+  <si>
+    <t>F6QG1G842P2KD</t>
+  </si>
+  <si>
+    <t>2FTS00067A</t>
+  </si>
+  <si>
+    <t>SAFEA2G60MA0F0A</t>
+  </si>
+  <si>
+    <t>2FTS00060A</t>
+  </si>
+  <si>
+    <t>F5QG942M5P2KB</t>
+  </si>
+  <si>
+    <t>2FTD00024A</t>
+  </si>
+  <si>
+    <t>D5PE942M5P3GT</t>
+  </si>
+  <si>
+    <t>2FTD00026A</t>
+  </si>
+  <si>
+    <t>D6HN1G842BN67</t>
+  </si>
+  <si>
+    <t>2FTS00069A</t>
+  </si>
+  <si>
+    <t>SAYRF1G95HN0F1B</t>
+  </si>
+  <si>
+    <t>2LL1N4BA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN1N4B02D</t>
+  </si>
+  <si>
+    <t>2INF00026A</t>
+  </si>
+  <si>
+    <t>LQP03TN0N7B02D</t>
+  </si>
+  <si>
+    <t>2CAC00812A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR50BA01*</t>
+  </si>
+  <si>
+    <t>2LL3N8BA11K-R</t>
+  </si>
+  <si>
+    <t>LQP03TN3N8B02D</t>
+  </si>
+  <si>
+    <t>2LL2N6BA11K-R</t>
+  </si>
+  <si>
+    <t>LQP03TN2N6B02D</t>
+  </si>
+  <si>
+    <t>2CAC00820A</t>
+  </si>
+  <si>
+    <t>GRM0335C1E3R0BA01D</t>
+  </si>
+  <si>
+    <t>2INF00023A</t>
+  </si>
+  <si>
+    <t>LQP03TN11NH02</t>
+  </si>
+  <si>
+    <t>2INF00021A</t>
+  </si>
+  <si>
+    <t>LQP03TN43NJ02D</t>
+  </si>
+  <si>
+    <t>2INF00024A</t>
+  </si>
+  <si>
+    <t>LQP03TN1N6B02D</t>
+  </si>
+  <si>
+    <t>2LP1N5BA50K-F</t>
+  </si>
+  <si>
+    <t>LQP03TN1N5B02D</t>
+  </si>
+  <si>
+    <t>2INF00025A</t>
+  </si>
+  <si>
+    <t>LQP03TN1N1B02D</t>
+  </si>
+  <si>
+    <t>2INF00022A</t>
+  </si>
+  <si>
+    <t>LQP03TN24NH02D</t>
+  </si>
+  <si>
+    <t>2CAC00815A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR20BA01D</t>
+  </si>
+  <si>
+    <t>2LL0N8BA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN0N8B02D</t>
+  </si>
+  <si>
+    <t>2LL3N9BA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN3N9B02D</t>
+  </si>
+  <si>
+    <t>2INF00020A</t>
+  </si>
+  <si>
+    <t>LQP03TN51NH02D</t>
+  </si>
+  <si>
+    <t>2LL8N2HA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN8N2H02D</t>
+  </si>
+  <si>
+    <t>2CAC00811A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR60BA01*</t>
+  </si>
+  <si>
+    <t>2CAC00814A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR30BA01D</t>
+  </si>
+  <si>
+    <t>2LP2N9BA50K-F</t>
+  </si>
+  <si>
+    <t>LQP03TN2N9B02D</t>
+  </si>
+  <si>
+    <t>2ICL00129A</t>
+  </si>
+  <si>
+    <t>SKY77753-51</t>
+  </si>
+  <si>
+    <t>2ICL00078A</t>
+  </si>
+  <si>
+    <t>SKY13399-468LF</t>
+  </si>
+  <si>
+    <t>2FTC00148A</t>
+  </si>
+  <si>
+    <t>LDM182G5010YC025</t>
+  </si>
+  <si>
+    <t>2CAC00869A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR70BA01</t>
+  </si>
+  <si>
+    <t>2LL2N1BA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN2N1B02D</t>
+  </si>
+  <si>
+    <t>2CAC00809A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H180GA01D</t>
+  </si>
+  <si>
+    <t>2CAC00803A</t>
+  </si>
+  <si>
+    <t>GRM033R61E104KE14</t>
+  </si>
+  <si>
+    <t>2CAC00813A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR40BA01D</t>
+  </si>
+  <si>
+    <t>2CAC00805A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H5R4BA01</t>
+  </si>
+  <si>
+    <t>2CAC00810A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H1R3BA01</t>
+  </si>
+  <si>
+    <t>2CAC00804A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H5R0BA01D</t>
   </si>
   <si>
     <t>2LL2N5BA11K-R</t>
@@ -744,10 +1137,10 @@
         <v>19</v>
       </c>
       <c r="H5" t="n">
-        <v>10.0</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I5" t="n">
-        <v>10.0</v>
+        <v>9840.0</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -776,16 +1169,16 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H6" t="n">
-        <v>1.2130000591278076</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I6" t="n">
-        <v>530.0</v>
+        <v>10000.0</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
@@ -805,22 +1198,22 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H7" t="n">
-        <v>0.210999995470047</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I7" t="n">
-        <v>3000.0</v>
+        <v>9975.0</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K7" t="s">
         <v>21</v>
@@ -840,22 +1233,22 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H8" t="n">
-        <v>351.1210021972656</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I8" t="n">
-        <v>4450.0</v>
+        <v>1934.0</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K8" t="s">
         <v>21</v>
@@ -875,22 +1268,22 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H9" t="n">
-        <v>53.21229934692383</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I9" t="n">
-        <v>2260.0</v>
+        <v>1950.0</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
         <v>21</v>
@@ -910,22 +1303,22 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H10" t="n">
-        <v>0.12309999763965607</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I10" t="n">
-        <v>768.0</v>
+        <v>12620.0</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K10" t="s">
         <v>21</v>
@@ -945,22 +1338,22 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H11" t="n">
-        <v>0.12399999797344208</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I11" t="n">
-        <v>1275.0</v>
+        <v>510.0</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K11" t="s">
         <v>21</v>
@@ -980,22 +1373,22 @@
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H12" t="n">
-        <v>0.352400004863739</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I12" t="n">
-        <v>2200.0</v>
+        <v>4247.0</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K12" t="s">
         <v>21</v>
@@ -1015,22 +1408,22 @@
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="H13" t="n">
-        <v>0.15600000321865082</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="I13" t="n">
-        <v>1560.0</v>
+        <v>2930.0</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K13" t="s">
         <v>21</v>
@@ -1050,24 +1443,2334 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I14" t="n">
+        <v>7260.0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I15" t="n">
+        <v>2200.0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
         <v>47</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H16" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I16" t="n">
+        <v>2127.0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
         <v>48</v>
       </c>
-      <c r="G14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.12300000339746475</v>
-      </c>
-      <c r="I14" t="n">
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2170.0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2180.0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1670.0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1712.0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1680.0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1610.0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1650.0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3660.0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I25" t="n">
+        <v>3790.0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I26" t="n">
+        <v>4300.0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I27" t="n">
+        <v>8980.0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I28" t="n">
+        <v>4480.0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I29" t="n">
+        <v>530.0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I30" t="n">
+        <v>3000.0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I31" t="n">
+        <v>4450.0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I32" t="n">
+        <v>2260.0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I33" t="n">
+        <v>768.0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1275.0</v>
+      </c>
+      <c r="J34" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2200.0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1560.0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I37" t="n">
+        <v>1330.0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1330.0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1020.0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I40" t="n">
+        <v>15830.0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" t="s">
+        <v>103</v>
+      </c>
+      <c r="G41" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I41" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>104</v>
+      </c>
+      <c r="F42" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I42" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I43" t="n">
+        <v>2710.0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I44" t="n">
+        <v>187.0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45" t="s">
+        <v>111</v>
+      </c>
+      <c r="G45" t="s">
+        <v>47</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I45" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="J45" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="s">
+        <v>112</v>
+      </c>
+      <c r="F46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I46" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>114</v>
+      </c>
+      <c r="F47" t="s">
+        <v>115</v>
+      </c>
+      <c r="G47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I47" t="n">
+        <v>4060.0</v>
+      </c>
+      <c r="J47" t="s">
+        <v>20</v>
+      </c>
+      <c r="K47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>116</v>
+      </c>
+      <c r="F48" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I48" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" t="s">
+        <v>118</v>
+      </c>
+      <c r="F49" t="s">
+        <v>119</v>
+      </c>
+      <c r="G49" t="s">
+        <v>19</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I49" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" t="s">
+        <v>120</v>
+      </c>
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I50" t="n">
+        <v>3300.0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>20</v>
+      </c>
+      <c r="K50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>122</v>
+      </c>
+      <c r="F51" t="s">
+        <v>123</v>
+      </c>
+      <c r="G51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I51" t="n">
+        <v>530.0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>20</v>
+      </c>
+      <c r="K51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>124</v>
+      </c>
+      <c r="F52" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1270.0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" t="s">
+        <v>126</v>
+      </c>
+      <c r="F53" t="s">
+        <v>127</v>
+      </c>
+      <c r="G53" t="s">
+        <v>19</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1430.0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>128</v>
+      </c>
+      <c r="F54" t="s">
+        <v>129</v>
+      </c>
+      <c r="G54" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I54" t="n">
+        <v>480.0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" t="s">
+        <v>130</v>
+      </c>
+      <c r="F55" t="s">
+        <v>131</v>
+      </c>
+      <c r="G55" t="s">
+        <v>19</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I55" t="n">
+        <v>530.0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>20</v>
+      </c>
+      <c r="K55" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" t="s">
+        <v>132</v>
+      </c>
+      <c r="F56" t="s">
+        <v>133</v>
+      </c>
+      <c r="G56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I56" t="n">
+        <v>530.0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" t="s">
+        <v>134</v>
+      </c>
+      <c r="F57" t="s">
+        <v>135</v>
+      </c>
+      <c r="G57" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I57" t="n">
+        <v>510.0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>20</v>
+      </c>
+      <c r="K57" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" t="s">
+        <v>137</v>
+      </c>
+      <c r="G58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I58" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" t="s">
+        <v>138</v>
+      </c>
+      <c r="F59" t="s">
+        <v>139</v>
+      </c>
+      <c r="G59" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I59" t="n">
+        <v>530.0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>20</v>
+      </c>
+      <c r="K59" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" t="s">
+        <v>140</v>
+      </c>
+      <c r="F60" t="s">
+        <v>141</v>
+      </c>
+      <c r="G60" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I60" t="n">
+        <v>3180.0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>20</v>
+      </c>
+      <c r="K60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" t="s">
+        <v>142</v>
+      </c>
+      <c r="F61" t="s">
+        <v>143</v>
+      </c>
+      <c r="G61" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I61" t="n">
+        <v>860.0</v>
+      </c>
+      <c r="J61" t="s">
+        <v>20</v>
+      </c>
+      <c r="K61" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" t="s">
+        <v>144</v>
+      </c>
+      <c r="F62" t="s">
+        <v>145</v>
+      </c>
+      <c r="G62" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I62" t="n">
+        <v>3090.0</v>
+      </c>
+      <c r="J62" t="s">
+        <v>20</v>
+      </c>
+      <c r="K62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" t="s">
+        <v>146</v>
+      </c>
+      <c r="F63" t="s">
+        <v>147</v>
+      </c>
+      <c r="G63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I63" t="n">
+        <v>540.0</v>
+      </c>
+      <c r="J63" t="s">
+        <v>20</v>
+      </c>
+      <c r="K63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" t="s">
+        <v>148</v>
+      </c>
+      <c r="F64" t="s">
+        <v>149</v>
+      </c>
+      <c r="G64" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I64" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>20</v>
+      </c>
+      <c r="K64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>150</v>
+      </c>
+      <c r="F65" t="s">
+        <v>151</v>
+      </c>
+      <c r="G65" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I65" t="n">
+        <v>16570.0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>20</v>
+      </c>
+      <c r="K65" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>152</v>
+      </c>
+      <c r="F66" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66" t="s">
+        <v>19</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I66" t="n">
+        <v>3530.0</v>
+      </c>
+      <c r="J66" t="s">
+        <v>20</v>
+      </c>
+      <c r="K66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" t="s">
+        <v>154</v>
+      </c>
+      <c r="F67" t="s">
+        <v>155</v>
+      </c>
+      <c r="G67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I67" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="J67" t="s">
+        <v>20</v>
+      </c>
+      <c r="K67" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" t="s">
+        <v>156</v>
+      </c>
+      <c r="F68" t="s">
+        <v>157</v>
+      </c>
+      <c r="G68" t="s">
+        <v>44</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I68" t="n">
+        <v>725.0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>20</v>
+      </c>
+      <c r="K68" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" t="s">
+        <v>158</v>
+      </c>
+      <c r="F69" t="s">
+        <v>159</v>
+      </c>
+      <c r="G69" t="s">
+        <v>44</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I69" t="n">
+        <v>1520.0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>20</v>
+      </c>
+      <c r="K69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" t="s">
+        <v>160</v>
+      </c>
+      <c r="F70" t="s">
+        <v>161</v>
+      </c>
+      <c r="G70" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I70" t="n">
         <v>4000.0</v>
       </c>
-      <c r="J14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="J70" t="s">
+        <v>20</v>
+      </c>
+      <c r="K70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" t="s">
+        <v>162</v>
+      </c>
+      <c r="F71" t="s">
+        <v>163</v>
+      </c>
+      <c r="G71" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I71" t="n">
+        <v>560.0</v>
+      </c>
+      <c r="J71" t="s">
+        <v>20</v>
+      </c>
+      <c r="K71" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" t="s">
+        <v>164</v>
+      </c>
+      <c r="F72" t="s">
+        <v>165</v>
+      </c>
+      <c r="G72" t="s">
+        <v>19</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I72" t="n">
+        <v>630.0</v>
+      </c>
+      <c r="J72" t="s">
+        <v>20</v>
+      </c>
+      <c r="K72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
+        <v>166</v>
+      </c>
+      <c r="F73" t="s">
+        <v>167</v>
+      </c>
+      <c r="G73" t="s">
+        <v>19</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I73" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="J73" t="s">
+        <v>20</v>
+      </c>
+      <c r="K73" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" t="s">
+        <v>168</v>
+      </c>
+      <c r="F74" t="s">
+        <v>169</v>
+      </c>
+      <c r="G74" t="s">
+        <v>19</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I74" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="J74" t="s">
+        <v>20</v>
+      </c>
+      <c r="K74" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" t="s">
+        <v>170</v>
+      </c>
+      <c r="F75" t="s">
+        <v>171</v>
+      </c>
+      <c r="G75" t="s">
+        <v>19</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I75" t="n">
+        <v>5520.0</v>
+      </c>
+      <c r="J75" t="s">
+        <v>20</v>
+      </c>
+      <c r="K75" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" t="s">
+        <v>172</v>
+      </c>
+      <c r="F76" t="s">
+        <v>173</v>
+      </c>
+      <c r="G76" t="s">
+        <v>19</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I76" t="n">
+        <v>3520.0</v>
+      </c>
+      <c r="J76" t="s">
+        <v>20</v>
+      </c>
+      <c r="K76" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" t="s">
+        <v>174</v>
+      </c>
+      <c r="F77" t="s">
+        <v>175</v>
+      </c>
+      <c r="G77" t="s">
+        <v>19</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I77" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="J77" t="s">
+        <v>20</v>
+      </c>
+      <c r="K77" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>176</v>
+      </c>
+      <c r="F78" t="s">
+        <v>177</v>
+      </c>
+      <c r="G78" t="s">
+        <v>19</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I78" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="J78" t="s">
+        <v>20</v>
+      </c>
+      <c r="K78" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79" t="s">
+        <v>178</v>
+      </c>
+      <c r="F79" t="s">
+        <v>179</v>
+      </c>
+      <c r="G79" t="s">
+        <v>19</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I79" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="J79" t="s">
+        <v>20</v>
+      </c>
+      <c r="K79" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80" t="s">
+        <v>178</v>
+      </c>
+      <c r="F80" t="s">
+        <v>179</v>
+      </c>
+      <c r="G80" t="s">
+        <v>19</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I80" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="J80" t="s">
+        <v>20</v>
+      </c>
+      <c r="K80" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add parts' info edit menu for shipper level
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/tempxls/개발자테스트아이디.xlsx
+++ b/src/main/webapp/resources/tempxls/개발자테스트아이디.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="200">
   <si>
     <t>LGIT P/N</t>
   </si>
@@ -63,10 +63,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>시작담당자</t>
+    <t>MSL Level</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>출고담당자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>TESTPRJA</t>
   </si>
   <si>
@@ -79,21 +83,45 @@
     <t>출고담당자시험용</t>
   </si>
   <si>
+    <t>AGAINEESS</t>
+  </si>
+  <si>
+    <t>MNAJH</t>
+  </si>
+  <si>
+    <t>399fdkAA</t>
+  </si>
+  <si>
+    <t>loapdlkj111</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>AGAINNEWAA</t>
+  </si>
+  <si>
+    <t>39fjdn2AA</t>
+  </si>
+  <si>
+    <t>MMGG</t>
+  </si>
+  <si>
+    <t>L432</t>
+  </si>
+  <si>
+    <t>384+2124</t>
+  </si>
+  <si>
     <t>NEWEXCELIM</t>
   </si>
   <si>
     <t>Hdidlfkje</t>
   </si>
   <si>
-    <t>MMGG</t>
-  </si>
-  <si>
-    <t>L432</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>LG19281NN</t>
   </si>
   <si>
@@ -103,12 +131,12 @@
     <t>MMMMAAAAABB</t>
   </si>
   <si>
-    <t>loapdlkj111</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
+    <t>2255+-9</t>
+  </si>
+  <si>
     <t>2CAC01209A</t>
   </si>
   <si>
@@ -121,10 +149,16 @@
     <t>S1</t>
   </si>
   <si>
+    <t>5,435</t>
+  </si>
+  <si>
     <t>2CAC01231A</t>
   </si>
   <si>
     <t>GRM0335C1H2R5BA01</t>
+  </si>
+  <si>
+    <t>20+-20</t>
   </si>
   <si>
     <t>2CAC01187A</t>
@@ -1068,19 +1102,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:K5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="4" customWidth="true" width="16.125" collapsed="false"/>
     <col min="5" max="5" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="10.0" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="9.5" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1126,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1098,7 +1134,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1106,7 +1142,7 @@
       <c r="F3" s="1"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="27">
+    <row r="4" spans="1:12" ht="27">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1153,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
@@ -1137,2773 +1173,3089 @@
       <c r="J4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" t="n">
-        <v>55.0</v>
+        <v>123.02300262451172</v>
       </c>
       <c r="I5" t="n">
-        <v>1055.0</v>
+        <v>50.0</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H6" t="n">
-        <v>123.0</v>
+        <v>55.0</v>
       </c>
       <c r="I6" t="n">
-        <v>456.0</v>
+        <v>1072.0</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
       <c r="H7" t="n">
-        <v>123.0</v>
+        <v>55.0</v>
       </c>
       <c r="I7" t="n">
-        <v>123.0</v>
+        <v>1072.0</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H8" t="n">
-        <v>0.10000000149011612</v>
+        <v>123.0</v>
       </c>
       <c r="I8" t="n">
-        <v>150.0</v>
+        <v>486.0</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K8" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H9" t="n">
-        <v>0.10000000149011612</v>
+        <v>123.0</v>
       </c>
       <c r="I9" t="n">
-        <v>9740.0</v>
+        <v>120.0</v>
       </c>
       <c r="J9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="L9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H10" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I10" t="n">
-        <v>9975.0</v>
+        <v>150.0</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>21</v>
+        <v>40</v>
+      </c>
+      <c r="L10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H11" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I11" t="n">
-        <v>1934.0</v>
+        <v>9740.0</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H12" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I12" t="n">
-        <v>1950.0</v>
+        <v>9975.0</v>
       </c>
       <c r="J12" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K12" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H13" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I13" t="n">
-        <v>12600.0</v>
+        <v>1934.0</v>
       </c>
       <c r="J13" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K13" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H14" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I14" t="n">
-        <v>510.0</v>
+        <v>1950.0</v>
       </c>
       <c r="J14" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K14" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="H15" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I15" t="n">
-        <v>4247.0</v>
+        <v>12600.0</v>
       </c>
       <c r="J15" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K15" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="H16" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I16" t="n">
-        <v>2930.0</v>
+        <v>510.0</v>
       </c>
       <c r="J16" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K16" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H17" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I17" t="n">
-        <v>7260.0</v>
+        <v>4247.0</v>
       </c>
       <c r="J17" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K17" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H18" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I18" t="n">
-        <v>2200.0</v>
+        <v>2930.0</v>
       </c>
       <c r="J18" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K18" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H19" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I19" t="n">
-        <v>2127.0</v>
+        <v>7260.0</v>
       </c>
       <c r="J19" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K19" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H20" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I20" t="n">
-        <v>2170.0</v>
+        <v>2200.0</v>
       </c>
       <c r="J20" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K20" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L20" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="H21" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I21" t="n">
-        <v>2180.0</v>
+        <v>2127.0</v>
       </c>
       <c r="J21" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K21" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L21" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G22" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H22" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I22" t="n">
-        <v>1670.0</v>
+        <v>2170.0</v>
       </c>
       <c r="J22" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K22" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L22" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="H23" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I23" t="n">
-        <v>1712.0</v>
+        <v>2180.0</v>
       </c>
       <c r="J23" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K23" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G24" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H24" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I24" t="n">
-        <v>1680.0</v>
+        <v>1670.0</v>
       </c>
       <c r="J24" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K24" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L24" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" t="s">
         <v>67</v>
       </c>
-      <c r="F25" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" t="s">
-        <v>56</v>
-      </c>
       <c r="H25" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I25" t="n">
-        <v>1610.0</v>
+        <v>1712.0</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K25" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H26" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I26" t="n">
-        <v>1650.0</v>
+        <v>1680.0</v>
       </c>
       <c r="J26" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K26" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L26" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H27" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I27" t="n">
-        <v>3660.0</v>
+        <v>1610.0</v>
       </c>
       <c r="J27" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K27" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L27" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="H28" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I28" t="n">
-        <v>3790.0</v>
+        <v>1650.0</v>
       </c>
       <c r="J28" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K28" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L28" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="G29" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H29" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I29" t="n">
-        <v>4300.0</v>
+        <v>3660.0</v>
       </c>
       <c r="J29" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K29" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L29" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="H30" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I30" t="n">
-        <v>8980.0</v>
+        <v>3790.0</v>
       </c>
       <c r="J30" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K30" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L30" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F31" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="H31" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I31" t="n">
-        <v>4480.0</v>
+        <v>4300.0</v>
       </c>
       <c r="J31" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K31" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L31" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G32" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="H32" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I32" t="n">
-        <v>530.0</v>
+        <v>8980.0</v>
       </c>
       <c r="J32" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K32" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L32" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F33" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G33" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H33" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I33" t="n">
-        <v>3000.0</v>
+        <v>4480.0</v>
       </c>
       <c r="J33" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K33" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L33" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="H34" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I34" t="n">
-        <v>4450.0</v>
+        <v>530.0</v>
       </c>
       <c r="J34" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K34" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L34" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="G35" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="H35" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I35" t="n">
-        <v>2260.0</v>
+        <v>3000.0</v>
       </c>
       <c r="J35" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K35" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L35" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F36" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" t="s">
         <v>93</v>
       </c>
-      <c r="G36" t="s">
-        <v>94</v>
-      </c>
       <c r="H36" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I36" t="n">
-        <v>768.0</v>
+        <v>4450.0</v>
       </c>
       <c r="J36" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K36" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L36" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G37" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="H37" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I37" t="n">
-        <v>1275.0</v>
+        <v>2260.0</v>
       </c>
       <c r="J37" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K37" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L37" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F38" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G38" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="H38" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I38" t="n">
-        <v>2200.0</v>
+        <v>768.0</v>
       </c>
       <c r="J38" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K38" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L38" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F39" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G39" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="H39" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I39" t="n">
-        <v>1560.0</v>
+        <v>1275.0</v>
       </c>
       <c r="J39" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K39" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="F40" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="G40" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="H40" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I40" t="n">
-        <v>1330.0</v>
+        <v>2200.0</v>
       </c>
       <c r="J40" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K40" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L40" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="F41" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="G41" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H41" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I41" t="n">
-        <v>1330.0</v>
+        <v>1560.0</v>
       </c>
       <c r="J41" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K41" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L41" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F42" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="G42" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H42" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I42" t="n">
-        <v>1020.0</v>
+        <v>1330.0</v>
       </c>
       <c r="J42" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K42" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L42" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F43" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="G43" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H43" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I43" t="n">
-        <v>15830.0</v>
+        <v>1330.0</v>
       </c>
       <c r="J43" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K43" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L43" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F44" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="G44" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H44" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I44" t="n">
-        <v>500.0</v>
+        <v>1020.0</v>
       </c>
       <c r="J44" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K44" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L44" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F45" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G45" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H45" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I45" t="n">
-        <v>19.0</v>
+        <v>15830.0</v>
       </c>
       <c r="J45" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K45" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L45" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="F46" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="G46" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="H46" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I46" t="n">
-        <v>2710.0</v>
+        <v>500.0</v>
       </c>
       <c r="J46" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K46" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L46" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F47" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="G47" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="H47" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I47" t="n">
-        <v>187.0</v>
+        <v>19.0</v>
       </c>
       <c r="J47" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K47" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L47" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F48" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G48" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H48" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I48" t="n">
-        <v>680.0</v>
+        <v>2710.0</v>
       </c>
       <c r="J48" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K48" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L48" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="F49" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="G49" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="H49" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I49" t="n">
-        <v>72.0</v>
+        <v>187.0</v>
       </c>
       <c r="J49" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K49" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L49" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F50" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G50" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H50" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I50" t="n">
-        <v>4060.0</v>
+        <v>680.0</v>
       </c>
       <c r="J50" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K50" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L50" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F51" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="G51" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H51" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I51" t="n">
-        <v>520.0</v>
+        <v>72.0</v>
       </c>
       <c r="J51" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K51" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L51" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F52" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="G52" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H52" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I52" t="n">
-        <v>520.0</v>
+        <v>4060.0</v>
       </c>
       <c r="J52" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K52" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L52" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="F53" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="G53" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H53" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I53" t="n">
-        <v>3300.0</v>
+        <v>520.0</v>
       </c>
       <c r="J53" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K53" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L53" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F54" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="G54" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H54" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I54" t="n">
-        <v>530.0</v>
+        <v>520.0</v>
       </c>
       <c r="J54" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K54" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L54" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F55" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="G55" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H55" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I55" t="n">
-        <v>1270.0</v>
+        <v>3300.0</v>
       </c>
       <c r="J55" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K55" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L55" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="F56" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="G56" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H56" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I56" t="n">
-        <v>1430.0</v>
+        <v>530.0</v>
       </c>
       <c r="J56" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K56" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L56" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="F57" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="G57" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H57" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I57" t="n">
-        <v>480.0</v>
+        <v>1270.0</v>
       </c>
       <c r="J57" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K57" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L57" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F58" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G58" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H58" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I58" t="n">
-        <v>530.0</v>
+        <v>1430.0</v>
       </c>
       <c r="J58" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K58" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L58" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F59" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="G59" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H59" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I59" t="n">
-        <v>530.0</v>
+        <v>480.0</v>
       </c>
       <c r="J59" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K59" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L59" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="F60" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="G60" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H60" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I60" t="n">
-        <v>510.0</v>
+        <v>530.0</v>
       </c>
       <c r="J60" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K60" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L60" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="F61" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G61" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H61" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I61" t="n">
-        <v>1000.0</v>
+        <v>530.0</v>
       </c>
       <c r="J61" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K61" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L61" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F62" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="G62" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H62" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I62" t="n">
-        <v>530.0</v>
+        <v>510.0</v>
       </c>
       <c r="J62" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K62" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L62" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C63" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F63" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="G63" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H63" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I63" t="n">
-        <v>3180.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J63" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K63" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L63" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D64" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="F64" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="G64" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H64" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I64" t="n">
-        <v>860.0</v>
+        <v>530.0</v>
       </c>
       <c r="J64" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K64" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L64" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C65" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D65" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="F65" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="G65" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H65" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I65" t="n">
-        <v>3090.0</v>
+        <v>3180.0</v>
       </c>
       <c r="J65" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K65" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L65" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F66" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="G66" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H66" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I66" t="n">
-        <v>540.0</v>
+        <v>860.0</v>
       </c>
       <c r="J66" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K66" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L66" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D67" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F67" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="G67" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H67" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I67" t="n">
-        <v>140.0</v>
+        <v>3090.0</v>
       </c>
       <c r="J67" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K67" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L67" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C68" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D68" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="F68" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G68" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H68" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I68" t="n">
-        <v>16570.0</v>
+        <v>540.0</v>
       </c>
       <c r="J68" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K68" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L68" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D69" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F69" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="G69" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H69" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I69" t="n">
-        <v>3530.0</v>
+        <v>140.0</v>
       </c>
       <c r="J69" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K69" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L69" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D70" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="F70" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="G70" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H70" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I70" t="n">
-        <v>1000.0</v>
+        <v>16570.0</v>
       </c>
       <c r="J70" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K70" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L70" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D71" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F71" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G71" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H71" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I71" t="n">
-        <v>725.0</v>
+        <v>3530.0</v>
       </c>
       <c r="J71" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K71" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L71" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="F72" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="G72" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H72" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I72" t="n">
-        <v>1520.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J72" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K72" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L72" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D73" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="F73" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="G73" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="H73" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I73" t="n">
-        <v>4000.0</v>
+        <v>725.0</v>
       </c>
       <c r="J73" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K73" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L73" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D74" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="F74" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="G74" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="H74" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I74" t="n">
-        <v>560.0</v>
+        <v>1520.0</v>
       </c>
       <c r="J74" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K74" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L74" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C75" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D75" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F75" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="G75" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H75" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I75" t="n">
-        <v>630.0</v>
+        <v>4000.0</v>
       </c>
       <c r="J75" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K75" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L75" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D76" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F76" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="G76" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H76" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I76" t="n">
-        <v>1000.0</v>
+        <v>560.0</v>
       </c>
       <c r="J76" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K76" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L76" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D77" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F77" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="G77" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H77" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I77" t="n">
-        <v>5000.0</v>
+        <v>630.0</v>
       </c>
       <c r="J77" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K77" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L77" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D78" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F78" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="G78" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H78" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I78" t="n">
-        <v>5520.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J78" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K78" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L78" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C79" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D79" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="F79" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="G79" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H79" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I79" t="n">
-        <v>3520.0</v>
+        <v>5000.0</v>
       </c>
       <c r="J79" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K79" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L79" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D80" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F80" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="G80" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H80" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I80" t="n">
-        <v>1000.0</v>
+        <v>5520.0</v>
       </c>
       <c r="J80" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K80" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L80" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D81" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="F81" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="G81" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H81" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I81" t="n">
-        <v>1000.0</v>
+        <v>3520.0</v>
       </c>
       <c r="J81" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K81" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L81" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C82" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D82" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E82" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F82" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="G82" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H82" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I82" t="n">
-        <v>4000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J82" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K82" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="L82" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D83" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E83" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="F83" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="G83" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H83" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I83" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="J83" t="s">
+        <v>39</v>
+      </c>
+      <c r="K83" t="s">
+        <v>43</v>
+      </c>
+      <c r="L83" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" t="s">
+        <v>198</v>
+      </c>
+      <c r="F84" t="s">
+        <v>199</v>
+      </c>
+      <c r="G84" t="s">
+        <v>38</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I84" t="n">
         <v>4000.0</v>
       </c>
-      <c r="J83" t="s">
-        <v>30</v>
-      </c>
-      <c r="K83" t="s">
-        <v>21</v>
+      <c r="J84" t="s">
+        <v>39</v>
+      </c>
+      <c r="K84" t="s">
+        <v>43</v>
+      </c>
+      <c r="L84" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" t="s">
+        <v>198</v>
+      </c>
+      <c r="F85" t="s">
+        <v>199</v>
+      </c>
+      <c r="G85" t="s">
+        <v>38</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I85" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="J85" t="s">
+        <v>39</v>
+      </c>
+      <c r="K85" t="s">
+        <v>43</v>
+      </c>
+      <c r="L85" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>